<commit_message>
Description not part name
</commit_message>
<xml_diff>
--- a/simInput.xlsx
+++ b/simInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saiakhilpulikam/Documents/GitHub/tariff-simulator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE93A73-3643-2E4D-B42D-C0B7D7E43950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C9ABD5F-1892-2B44-92CB-EFF3D3FF0836}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="640" windowWidth="29280" windowHeight="21700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -392,16 +392,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -453,11 +445,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -765,7 +757,7 @@
   <dimension ref="A1:T51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -792,3105 +784,3106 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" t="s">
+      <c r="D2" s="1"/>
+      <c r="E2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="3">
         <v>12</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="3">
         <v>19.66</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="3">
         <v>1.06</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="3">
         <v>0.22</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="3">
         <v>20</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="3">
         <v>4261</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="3">
         <v>105979.592</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="3">
         <v>202</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="3">
         <v>15</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="3">
         <v>89</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="3">
         <v>1275</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="3">
         <v>0.34</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="3">
         <v>0.23</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="3">
         <v>0.33</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" t="s">
+      <c r="D3" s="1"/>
+      <c r="E3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="3">
         <v>26</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="3">
         <v>7.55</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="3">
         <v>1.4</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="3">
         <v>1.39</v>
       </c>
-      <c r="K3">
+      <c r="K3" s="3">
         <v>50</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="3">
         <v>8314</v>
       </c>
-      <c r="M3">
+      <c r="M3" s="3">
         <v>117352.11</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="3">
         <v>535</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="3">
         <v>10</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="3">
         <v>93</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="3">
         <v>534</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="3">
         <v>0.31</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="3">
         <v>0.28000000000000003</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="3">
         <v>0.26</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="3"/>
-      <c r="E4" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="3">
         <v>32</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="3">
         <v>6.74</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="3">
         <v>0.56000000000000005</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="3">
         <v>6.89</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="3">
         <v>25</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="3">
         <v>23442</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="3">
         <v>372141.75</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="3">
         <v>960</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="3">
         <v>15</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="3">
         <v>86</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="3">
         <v>2753</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="3">
         <v>0.27</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="3">
         <v>0.47</v>
       </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D5" s="3"/>
-      <c r="E5" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="3">
         <v>26</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="3">
         <v>7.27</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="3">
         <v>1.0900000000000001</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="3">
         <v>4.01</v>
       </c>
-      <c r="K5">
+      <c r="K5" s="3">
         <v>50</v>
       </c>
-      <c r="L5">
+      <c r="L5" s="3">
         <v>35502</v>
       </c>
-      <c r="M5">
+      <c r="M5" s="3">
         <v>568209.51</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="3">
         <v>370</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="3">
         <v>15</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="3">
         <v>94</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="3">
         <v>2455</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="3">
         <v>0.23</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="3">
         <v>0.19</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="3">
         <v>0.34</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" t="s">
+      <c r="D6" s="1"/>
+      <c r="E6" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="3">
         <v>32</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="3">
         <v>10.130000000000001</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
         <v>0.97</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="3">
         <v>1.59</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="3">
         <v>25</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="3">
         <v>48007</v>
       </c>
-      <c r="M6">
+      <c r="M6" s="3">
         <v>730786.55750000011</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="3">
         <v>206</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="3">
         <v>15</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="3">
         <v>77</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="3">
         <v>2085</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="3">
         <v>0.25</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="3">
         <v>0.12</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="3">
         <v>0.37</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" t="s">
+      <c r="D7" s="1"/>
+      <c r="E7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="3">
         <v>32</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="3">
         <v>5.22</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="3">
         <v>1.1200000000000001</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="3">
         <v>1.58</v>
       </c>
-      <c r="K7">
+      <c r="K7" s="3">
         <v>25</v>
       </c>
-      <c r="L7">
+      <c r="L7" s="3">
         <v>13165</v>
       </c>
-      <c r="M7">
+      <c r="M7" s="3">
         <v>121447.125</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="3">
         <v>171</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="3">
         <v>15</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="3">
         <v>79</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="3">
         <v>1521</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="3">
         <v>0.34</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="3">
         <v>0.17</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="3">
         <v>0.41</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D8" s="3"/>
-      <c r="E8" t="s">
+      <c r="D8" s="1"/>
+      <c r="E8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="3">
         <v>32</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="3">
         <v>4.09</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="3">
         <v>0.86</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="3">
         <v>1.21</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="3">
         <v>25</v>
       </c>
-      <c r="L8">
+      <c r="L8" s="3">
         <v>33876</v>
       </c>
-      <c r="M8">
+      <c r="M8" s="3">
         <v>243314.37</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="3">
         <v>800</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="3">
         <v>10</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="3">
         <v>93</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="3">
         <v>1629</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="3">
         <v>0.25</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="3">
         <v>0.23</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="3">
         <v>0.24</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D9" s="3"/>
-      <c r="E9" t="s">
+      <c r="D9" s="1"/>
+      <c r="E9" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="3">
         <v>32</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="3">
         <v>14.18</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="3">
         <v>0.68</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="3">
         <v>8.02</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="3">
         <v>25</v>
       </c>
-      <c r="L9">
+      <c r="L9" s="3">
         <v>40960</v>
       </c>
-      <c r="M9">
+      <c r="M9" s="3">
         <v>1082368</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="3">
         <v>120</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="3">
         <v>10</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="3">
         <v>81</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="3">
         <v>2000</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="3">
         <v>0.17</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="3">
         <v>0.23</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="3">
         <v>0.38</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" t="s">
+      <c r="D10" s="1"/>
+      <c r="E10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="3">
         <v>12</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="3">
         <v>6.75</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="3">
         <v>1.25</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="3">
         <v>2.84</v>
       </c>
-      <c r="K10">
+      <c r="K10" s="3">
         <v>20</v>
       </c>
-      <c r="L10">
+      <c r="L10" s="3">
         <v>12994</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="3">
         <v>158396.85999999999</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="3">
         <v>714</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="3">
         <v>15</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="3">
         <v>83</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="3">
         <v>1202</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="3">
         <v>0.17</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="3">
         <v>0.22</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="3">
         <v>0.36</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" t="s">
+      <c r="D11" s="1"/>
+      <c r="E11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="3">
         <v>32</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="3">
         <v>14.96</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="3">
         <v>0.66</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="3">
         <v>3.5</v>
       </c>
-      <c r="K11">
+      <c r="K11" s="3">
         <v>25</v>
       </c>
-      <c r="L11">
+      <c r="L11" s="3">
         <v>20324</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="3">
         <v>464606.64000000007</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="3">
         <v>221</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="3">
         <v>15</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="3">
         <v>81</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="3">
         <v>2949</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="3">
         <v>0.15</v>
       </c>
-      <c r="T11">
+      <c r="T11" s="3">
         <v>0.26</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" t="s">
+      <c r="D12" s="1"/>
+      <c r="E12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="3">
         <v>12</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="3">
         <v>7.4</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="3">
         <v>0.98</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="3">
         <v>3.34</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="3">
         <v>20</v>
       </c>
-      <c r="L12">
+      <c r="L12" s="3">
         <v>15885</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="3">
         <v>209682</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="3">
         <v>566</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="3">
         <v>10</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="3">
         <v>92</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="3">
         <v>2079</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="3">
         <v>0.1</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="3">
         <v>0.21</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="3">
         <v>0.48</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="D13" s="3"/>
-      <c r="E13" t="s">
+      <c r="D13" s="1"/>
+      <c r="E13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="3">
         <v>12</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="3">
         <v>13.37</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="3">
         <v>0.85</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="3">
         <v>0.22</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="3">
         <v>20</v>
       </c>
-      <c r="L13">
+      <c r="L13" s="3">
         <v>13195</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="3">
         <v>225819.23</v>
       </c>
-      <c r="N13">
+      <c r="N13" s="3">
         <v>314</v>
       </c>
-      <c r="O13">
+      <c r="O13" s="3">
         <v>10</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="3">
         <v>78</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="3">
         <v>661</v>
       </c>
-      <c r="R13">
+      <c r="R13" s="3">
         <v>0.21</v>
       </c>
-      <c r="S13">
+      <c r="S13" s="3">
         <v>0.18</v>
       </c>
-      <c r="T13">
+      <c r="T13" s="3">
         <v>0.38</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D14" s="3"/>
-      <c r="E14" t="s">
+      <c r="D14" s="1"/>
+      <c r="E14" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="3">
         <v>32</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="3">
         <v>8.16</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="3">
         <v>1</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="3">
         <v>3.93</v>
       </c>
-      <c r="K14">
+      <c r="K14" s="3">
         <v>25</v>
       </c>
-      <c r="L14">
+      <c r="L14" s="3">
         <v>41764</v>
       </c>
-      <c r="M14">
+      <c r="M14" s="3">
         <v>631889.32000000007</v>
       </c>
-      <c r="N14">
+      <c r="N14" s="3">
         <v>430</v>
       </c>
-      <c r="O14">
+      <c r="O14" s="3">
         <v>10</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="3">
         <v>88</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="3">
         <v>701</v>
       </c>
-      <c r="R14">
+      <c r="R14" s="3">
         <v>0.2</v>
       </c>
-      <c r="S14">
+      <c r="S14" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="T14">
+      <c r="T14" s="3">
         <v>0.41</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" t="s">
+      <c r="D15" s="1"/>
+      <c r="E15" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="3">
         <v>12</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="3">
         <v>6.69</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="3">
         <v>0.67</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="K15">
+      <c r="K15" s="3">
         <v>20</v>
       </c>
-      <c r="L15">
+      <c r="L15" s="3">
         <v>15564</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="3">
         <v>139889.23199999999</v>
       </c>
-      <c r="N15">
+      <c r="N15" s="3">
         <v>558</v>
       </c>
-      <c r="O15">
+      <c r="O15" s="3">
         <v>20</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="3">
         <v>92</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="3">
         <v>2481</v>
       </c>
-      <c r="R15">
+      <c r="R15" s="3">
         <v>0.17</v>
       </c>
-      <c r="S15">
+      <c r="S15" s="3">
         <v>0.27</v>
       </c>
-      <c r="T15">
+      <c r="T15" s="3">
         <v>0.46</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="3">
         <v>84189990</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="3">
         <v>32</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="3">
         <v>5.58</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="3">
         <v>1.27</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="3">
         <v>9.48</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="3">
         <v>25</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="3">
         <v>12695</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="3">
         <v>225018.875</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="3">
         <v>187</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="3">
         <v>20</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="3">
         <v>83</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="3">
         <v>1495</v>
       </c>
-      <c r="R16">
+      <c r="R16" s="3">
         <v>0.1</v>
       </c>
-      <c r="S16">
+      <c r="S16" s="3">
         <v>0.24</v>
       </c>
-      <c r="T16">
+      <c r="T16" s="3">
         <v>0.39</v>
       </c>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="3" t="s">
+      <c r="C17" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" t="s">
+      <c r="D17" s="1"/>
+      <c r="E17" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="3">
         <v>26</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="3">
         <v>10.57</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="3">
         <v>0.81</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="3">
         <v>7.45</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="3">
         <v>50</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="3">
         <v>8899</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="3">
         <v>214599.38500000001</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="3">
         <v>472</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="3">
         <v>20</v>
       </c>
-      <c r="P17">
+      <c r="P17" s="3">
         <v>76</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="3">
         <v>2817</v>
       </c>
-      <c r="R17">
+      <c r="R17" s="3">
         <v>0.15</v>
       </c>
-      <c r="S17">
+      <c r="S17" s="3">
         <v>0.15</v>
       </c>
-      <c r="T17">
+      <c r="T17" s="3">
         <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C18" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="3">
         <v>84189990</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="3">
         <v>32</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="3">
         <v>13.32</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="3">
         <v>1.44</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="3">
         <v>0.95</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="3">
         <v>25</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="3">
         <v>23155</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="3">
         <v>440871.20000000013</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="3">
         <v>199</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="3">
         <v>15</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="3">
         <v>94</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="3">
         <v>1315</v>
       </c>
-      <c r="R18">
+      <c r="R18" s="3">
         <v>0.28000000000000003</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="3">
         <v>0.15</v>
       </c>
-      <c r="T18">
+      <c r="T18" s="3">
         <v>0.23</v>
       </c>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="A19" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="1">
         <v>84189990</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="3">
         <v>26</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="3">
         <v>4.4800000000000004</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="3">
         <v>1.49</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="3">
         <v>6.51</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="3">
         <v>50</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="3">
         <v>36429</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="3">
         <v>536234.88</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="3">
         <v>971</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="3">
         <v>20</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="3">
         <v>89</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="3">
         <v>955</v>
       </c>
-      <c r="R19">
+      <c r="R19" s="3">
         <v>0.3</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="3">
         <v>0.11</v>
       </c>
-      <c r="T19">
+      <c r="T19" s="3">
         <v>0.34</v>
       </c>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="1">
         <v>84189990</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="3">
         <v>26</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="3">
         <v>7.87</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="3">
         <v>1</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="3">
         <v>1.98</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="3">
         <v>50</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="3">
         <v>20504</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="3">
         <v>303151.64</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="3">
         <v>763</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="3">
         <v>15</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="3">
         <v>81</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="3">
         <v>1775</v>
       </c>
-      <c r="R20">
+      <c r="R20" s="3">
         <v>0.25</v>
       </c>
-      <c r="S20">
+      <c r="S20" s="3">
         <v>0.24</v>
       </c>
-      <c r="T20">
+      <c r="T20" s="3">
         <v>0.27</v>
       </c>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="3">
         <v>32</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="3">
         <v>3.05</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="3">
         <v>0.97</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="3">
         <v>2.95</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="3">
         <v>25</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="3">
         <v>5948</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="3">
         <v>45992.91</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="3">
         <v>230</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="3">
         <v>15</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="3">
         <v>86</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="3">
         <v>1516</v>
       </c>
-      <c r="R21">
+      <c r="R21" s="3">
         <v>0.33</v>
       </c>
-      <c r="S21">
+      <c r="S21" s="3">
         <v>0.12</v>
       </c>
-      <c r="T21">
+      <c r="T21" s="3">
         <v>0.32</v>
       </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="3">
         <v>84189990</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="3">
         <v>12</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="3">
         <v>17.14</v>
       </c>
-      <c r="I22" s="2">
+      <c r="I22" s="3">
         <v>1.05</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" s="3">
         <v>0.9</v>
       </c>
-      <c r="K22" s="2">
+      <c r="K22" s="3">
         <v>20</v>
       </c>
-      <c r="L22" s="2">
+      <c r="L22" s="3">
         <v>17876</v>
       </c>
-      <c r="M22" s="2">
+      <c r="M22" s="3">
         <v>402531.76799999998</v>
       </c>
-      <c r="N22">
+      <c r="N22" s="3">
         <v>213</v>
       </c>
-      <c r="O22">
+      <c r="O22" s="3">
         <v>20</v>
       </c>
-      <c r="P22">
+      <c r="P22" s="3">
         <v>90</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" s="3">
         <v>573</v>
       </c>
-      <c r="R22">
+      <c r="R22" s="3">
         <v>0.2</v>
       </c>
-      <c r="S22">
+      <c r="S22" s="3">
         <v>0.23</v>
       </c>
-      <c r="T22">
+      <c r="T22" s="3">
         <v>0.3</v>
       </c>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <v>84189990</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="3">
         <v>32</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="3">
         <v>9.56</v>
       </c>
-      <c r="I23" s="2">
+      <c r="I23" s="3">
         <v>1.37</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="3">
         <v>10.69</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="3">
         <v>25</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L23" s="3">
         <v>39498</v>
       </c>
-      <c r="M23" s="2">
+      <c r="M23" s="3">
         <v>948346.98</v>
       </c>
-      <c r="N23">
+      <c r="N23" s="3">
         <v>422</v>
       </c>
-      <c r="O23">
+      <c r="O23" s="3">
         <v>10</v>
       </c>
-      <c r="P23">
+      <c r="P23" s="3">
         <v>90</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="3">
         <v>2481</v>
       </c>
-      <c r="R23">
+      <c r="R23" s="3">
         <v>0.31</v>
       </c>
-      <c r="S23">
+      <c r="S23" s="3">
         <v>0.24</v>
       </c>
-      <c r="T23">
+      <c r="T23" s="3">
         <v>0.38</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2" t="s">
+      <c r="D24" s="3"/>
+      <c r="E24" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="3">
         <v>26</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="3">
         <v>8.9700000000000006</v>
       </c>
-      <c r="I24" s="2">
+      <c r="I24" s="3">
         <v>1.0900000000000001</v>
       </c>
-      <c r="J24" s="2">
+      <c r="J24" s="3">
         <v>4.67</v>
       </c>
-      <c r="K24" s="2">
+      <c r="K24" s="3">
         <v>50</v>
       </c>
-      <c r="L24" s="2">
+      <c r="L24" s="3">
         <v>20159</v>
       </c>
-      <c r="M24" s="2">
+      <c r="M24" s="3">
         <v>387355.185</v>
       </c>
-      <c r="N24">
+      <c r="N24" s="3">
         <v>937</v>
       </c>
-      <c r="O24">
+      <c r="O24" s="3">
         <v>10</v>
       </c>
-      <c r="P24">
+      <c r="P24" s="3">
         <v>86</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="3">
         <v>1942</v>
       </c>
-      <c r="R24">
+      <c r="R24" s="3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="S24">
+      <c r="S24" s="3">
         <v>0.13</v>
       </c>
-      <c r="T24">
+      <c r="T24" s="3">
         <v>0.22</v>
       </c>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="3">
         <v>32</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="3">
         <v>11.52</v>
       </c>
-      <c r="I25" s="2">
+      <c r="I25" s="3">
         <v>1.47</v>
       </c>
-      <c r="J25" s="2">
+      <c r="J25" s="3">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K25" s="2">
+      <c r="K25" s="3">
         <v>25</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L25" s="3">
         <v>38261</v>
       </c>
-      <c r="M25" s="2">
+      <c r="M25" s="3">
         <v>649289.16999999899</v>
       </c>
-      <c r="N25">
+      <c r="N25" s="3">
         <v>355</v>
       </c>
-      <c r="O25">
+      <c r="O25" s="3">
         <v>10</v>
       </c>
-      <c r="P25">
+      <c r="P25" s="3">
         <v>82</v>
       </c>
-      <c r="Q25">
+      <c r="Q25" s="3">
         <v>1450</v>
       </c>
-      <c r="R25">
+      <c r="R25" s="3">
         <v>0.16</v>
       </c>
-      <c r="S25">
+      <c r="S25" s="3">
         <v>0.2</v>
       </c>
-      <c r="T25">
+      <c r="T25" s="3">
         <v>0.5</v>
       </c>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2" t="s">
+      <c r="D26" s="3"/>
+      <c r="E26" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="3">
         <v>26</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="3">
         <v>2.91</v>
       </c>
-      <c r="I26" s="2">
+      <c r="I26" s="3">
         <v>0.53</v>
       </c>
-      <c r="J26" s="2">
+      <c r="J26" s="3">
         <v>4.43</v>
       </c>
-      <c r="K26" s="2">
+      <c r="K26" s="3">
         <v>50</v>
       </c>
-      <c r="L26" s="2">
+      <c r="L26" s="3">
         <v>7573</v>
       </c>
-      <c r="M26" s="2">
+      <c r="M26" s="3">
         <v>70618.224999999904</v>
       </c>
-      <c r="N26">
+      <c r="N26" s="3">
         <v>615</v>
       </c>
-      <c r="O26">
+      <c r="O26" s="3">
         <v>15</v>
       </c>
-      <c r="P26">
+      <c r="P26" s="3">
         <v>82</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="3">
         <v>2013</v>
       </c>
-      <c r="R26">
+      <c r="R26" s="3">
         <v>0.17</v>
       </c>
-      <c r="S26">
+      <c r="S26" s="3">
         <v>0.27</v>
       </c>
-      <c r="T26">
+      <c r="T26" s="3">
         <v>0.28000000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="3">
         <v>9025.19</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="3">
         <v>32</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="3">
         <v>8.31</v>
       </c>
-      <c r="I27" s="2">
+      <c r="I27" s="3">
         <v>0.71</v>
       </c>
-      <c r="J27" s="2">
+      <c r="J27" s="3">
         <v>5.72</v>
       </c>
-      <c r="K27" s="2">
+      <c r="K27" s="3">
         <v>25</v>
       </c>
-      <c r="L27" s="2">
+      <c r="L27" s="3">
         <v>6385</v>
       </c>
-      <c r="M27" s="2">
+      <c r="M27" s="3">
         <v>107379.737499999</v>
       </c>
-      <c r="N27">
+      <c r="N27" s="3">
         <v>978</v>
       </c>
-      <c r="O27">
+      <c r="O27" s="3">
         <v>20</v>
       </c>
-      <c r="P27">
+      <c r="P27" s="3">
         <v>78</v>
       </c>
-      <c r="Q27">
+      <c r="Q27" s="3">
         <v>599</v>
       </c>
-      <c r="R27">
+      <c r="R27" s="3">
         <v>0.35</v>
       </c>
-      <c r="S27">
+      <c r="S27" s="3">
         <v>0.2</v>
       </c>
-      <c r="T27">
+      <c r="T27" s="3">
         <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="3">
         <v>9032.1</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="3">
         <v>12</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="3">
         <v>8.14</v>
       </c>
-      <c r="I28" s="2">
+      <c r="I28" s="3">
         <v>0.88</v>
       </c>
-      <c r="J28" s="2">
+      <c r="J28" s="3">
         <v>0.28000000000000003</v>
       </c>
-      <c r="K28" s="2">
+      <c r="K28" s="3">
         <v>20</v>
       </c>
-      <c r="L28" s="2">
+      <c r="L28" s="3">
         <v>5446</v>
       </c>
-      <c r="M28" s="2">
+      <c r="M28" s="3">
         <v>59513.887999999999</v>
       </c>
-      <c r="N28">
+      <c r="N28" s="3">
         <v>936</v>
       </c>
-      <c r="O28">
+      <c r="O28" s="3">
         <v>20</v>
       </c>
-      <c r="P28">
+      <c r="P28" s="3">
         <v>82</v>
       </c>
-      <c r="Q28">
+      <c r="Q28" s="3">
         <v>2010</v>
       </c>
-      <c r="R28">
+      <c r="R28" s="3">
         <v>0.19</v>
       </c>
-      <c r="S28">
+      <c r="S28" s="3">
         <v>0.11</v>
       </c>
-      <c r="T28">
+      <c r="T28" s="3">
         <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="E29" s="2" t="s">
+      <c r="E29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="3">
         <v>12</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="3">
         <v>18.75</v>
       </c>
-      <c r="I29" s="2">
+      <c r="I29" s="3">
         <v>0.86</v>
       </c>
-      <c r="J29" s="2">
+      <c r="J29" s="3">
         <v>1.44</v>
       </c>
-      <c r="K29" s="2">
+      <c r="K29" s="3">
         <v>20</v>
       </c>
-      <c r="L29" s="2">
+      <c r="L29" s="3">
         <v>11221</v>
       </c>
-      <c r="M29" s="2">
+      <c r="M29" s="3">
         <v>278280.8</v>
       </c>
-      <c r="N29">
+      <c r="N29" s="3">
         <v>477</v>
       </c>
-      <c r="O29">
+      <c r="O29" s="3">
         <v>10</v>
       </c>
-      <c r="P29">
+      <c r="P29" s="3">
         <v>88</v>
       </c>
-      <c r="Q29">
+      <c r="Q29" s="3">
         <v>577</v>
       </c>
-      <c r="R29">
+      <c r="R29" s="3">
         <v>0.27</v>
       </c>
-      <c r="S29">
+      <c r="S29" s="3">
         <v>0.12</v>
       </c>
-      <c r="T29">
+      <c r="T29" s="3">
         <v>0.24</v>
       </c>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2" t="s">
+      <c r="D30" s="3"/>
+      <c r="E30" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="3">
         <v>12</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="3">
         <v>6.37</v>
       </c>
-      <c r="I30" s="2">
+      <c r="I30" s="3">
         <v>1.03</v>
       </c>
-      <c r="J30" s="2">
+      <c r="J30" s="3">
         <v>2.82</v>
       </c>
-      <c r="K30" s="2">
+      <c r="K30" s="3">
         <v>20</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L30" s="3">
         <v>5337</v>
       </c>
-      <c r="M30" s="2">
+      <c r="M30" s="3">
         <v>61343.478000000003</v>
       </c>
-      <c r="N30">
+      <c r="N30" s="3">
         <v>863</v>
       </c>
-      <c r="O30">
+      <c r="O30" s="3">
         <v>15</v>
       </c>
-      <c r="P30">
+      <c r="P30" s="3">
         <v>84</v>
       </c>
-      <c r="Q30">
+      <c r="Q30" s="3">
         <v>1730</v>
       </c>
-      <c r="R30">
+      <c r="R30" s="3">
         <v>0.2</v>
       </c>
-      <c r="S30">
+      <c r="S30" s="3">
         <v>0.11</v>
       </c>
-      <c r="T30">
+      <c r="T30" s="3">
         <v>0.34</v>
       </c>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E31" s="2" t="s">
+      <c r="D31" s="3"/>
+      <c r="E31" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" s="3">
         <v>26</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="3">
         <v>9.6</v>
       </c>
-      <c r="I31" s="2">
+      <c r="I31" s="3">
         <v>0.59</v>
       </c>
-      <c r="J31" s="2">
+      <c r="J31" s="3">
         <v>9.06</v>
       </c>
-      <c r="K31" s="2">
+      <c r="K31" s="3">
         <v>50</v>
       </c>
-      <c r="L31" s="2">
+      <c r="L31" s="3">
         <v>15782</v>
       </c>
-      <c r="M31" s="2">
+      <c r="M31" s="3">
         <v>379557.1</v>
       </c>
-      <c r="N31">
+      <c r="N31" s="3">
         <v>786</v>
       </c>
-      <c r="O31">
+      <c r="O31" s="3">
         <v>20</v>
       </c>
-      <c r="P31">
+      <c r="P31" s="3">
         <v>84</v>
       </c>
-      <c r="Q31">
+      <c r="Q31" s="3">
         <v>2231</v>
       </c>
-      <c r="R31">
+      <c r="R31" s="3">
         <v>0.28000000000000003</v>
       </c>
-      <c r="S31">
+      <c r="S31" s="3">
         <v>0.2</v>
       </c>
-      <c r="T31">
+      <c r="T31" s="3">
         <v>0.31</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="3">
         <v>84189900</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="3">
         <v>12</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="3">
         <v>12.08</v>
       </c>
-      <c r="I32" s="2">
+      <c r="I32" s="3">
         <v>1.19</v>
       </c>
-      <c r="J32" s="2">
+      <c r="J32" s="3">
         <v>0.28000000000000003</v>
       </c>
-      <c r="K32" s="2">
+      <c r="K32" s="3">
         <v>20</v>
       </c>
-      <c r="L32" s="2">
+      <c r="L32" s="3">
         <v>7725</v>
       </c>
-      <c r="M32" s="2">
+      <c r="M32" s="3">
         <v>123337.35</v>
       </c>
-      <c r="N32">
+      <c r="N32" s="3">
         <v>532</v>
       </c>
-      <c r="O32">
+      <c r="O32" s="3">
         <v>10</v>
       </c>
-      <c r="P32">
+      <c r="P32" s="3">
         <v>79</v>
       </c>
-      <c r="Q32">
+      <c r="Q32" s="3">
         <v>825</v>
       </c>
-      <c r="R32">
+      <c r="R32" s="3">
         <v>0.3</v>
       </c>
-      <c r="S32">
+      <c r="S32" s="3">
         <v>0.15</v>
       </c>
-      <c r="T32">
+      <c r="T32" s="3">
         <v>0.22</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="3">
         <v>8501.1</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" s="3">
         <v>32</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="3">
         <v>4.1900000000000004</v>
       </c>
-      <c r="I33" s="2">
+      <c r="I33" s="3">
         <v>1.19</v>
       </c>
-      <c r="J33" s="2">
+      <c r="J33" s="3">
         <v>1.45</v>
       </c>
-      <c r="K33" s="2">
+      <c r="K33" s="3">
         <v>25</v>
       </c>
-      <c r="L33" s="2">
+      <c r="L33" s="3">
         <v>22667</v>
       </c>
-      <c r="M33" s="2">
+      <c r="M33" s="3">
         <v>178559.29250000001</v>
       </c>
-      <c r="N33">
+      <c r="N33" s="3">
         <v>891</v>
       </c>
-      <c r="O33">
+      <c r="O33" s="3">
         <v>20</v>
       </c>
-      <c r="P33">
+      <c r="P33" s="3">
         <v>80</v>
       </c>
-      <c r="Q33">
+      <c r="Q33" s="3">
         <v>1355</v>
       </c>
-      <c r="R33">
+      <c r="R33" s="3">
         <v>0.2</v>
       </c>
-      <c r="S33">
+      <c r="S33" s="3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="T33">
+      <c r="T33" s="3">
         <v>0.35</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="3">
         <v>84189990</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="3">
         <v>12</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="3">
         <v>15.47</v>
       </c>
-      <c r="I34" s="2">
+      <c r="I34" s="3">
         <v>1.1599999999999999</v>
       </c>
-      <c r="J34" s="2">
+      <c r="J34" s="3">
         <v>2.81</v>
       </c>
-      <c r="K34" s="2">
+      <c r="K34" s="3">
         <v>20</v>
       </c>
-      <c r="L34" s="2">
+      <c r="L34" s="3">
         <v>15729</v>
       </c>
-      <c r="M34" s="2">
+      <c r="M34" s="3">
         <v>354437.28600000002</v>
       </c>
-      <c r="N34">
+      <c r="N34" s="3">
         <v>325</v>
       </c>
-      <c r="O34">
+      <c r="O34" s="3">
         <v>20</v>
       </c>
-      <c r="P34">
+      <c r="P34" s="3">
         <v>81</v>
       </c>
-      <c r="Q34">
+      <c r="Q34" s="3">
         <v>2685</v>
       </c>
-      <c r="R34">
+      <c r="R34" s="3">
         <v>0.33</v>
       </c>
-      <c r="S34">
+      <c r="S34" s="3">
         <v>0.25</v>
       </c>
-      <c r="T34">
+      <c r="T34" s="3">
         <v>0.37</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="2" t="s">
+      <c r="D35" s="1"/>
+      <c r="E35" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" s="3">
         <v>26</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="3">
         <v>7.01</v>
       </c>
-      <c r="I35" s="2">
+      <c r="I35" s="3">
         <v>1.35</v>
       </c>
-      <c r="J35" s="2">
+      <c r="J35" s="3">
         <v>8.91</v>
       </c>
-      <c r="K35" s="2">
+      <c r="K35" s="3">
         <v>50</v>
       </c>
-      <c r="L35" s="2">
+      <c r="L35" s="3">
         <v>17554</v>
       </c>
-      <c r="M35" s="2">
+      <c r="M35" s="3">
         <v>364684.35</v>
       </c>
-      <c r="N35">
+      <c r="N35" s="3">
         <v>972</v>
       </c>
-      <c r="O35">
+      <c r="O35" s="3">
         <v>15</v>
       </c>
-      <c r="P35">
+      <c r="P35" s="3">
         <v>89</v>
       </c>
-      <c r="Q35">
+      <c r="Q35" s="3">
         <v>1424</v>
       </c>
-      <c r="R35">
+      <c r="R35" s="3">
         <v>0.13</v>
       </c>
-      <c r="S35">
+      <c r="S35" s="3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="T35">
+      <c r="T35" s="3">
         <v>0.44</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="C36" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36" s="3">
         <v>12</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="3">
         <v>15.82</v>
       </c>
-      <c r="I36" s="2">
+      <c r="I36" s="3">
         <v>1.1399999999999999</v>
       </c>
-      <c r="J36" s="2">
+      <c r="J36" s="3">
         <v>0.41</v>
       </c>
-      <c r="K36" s="2">
+      <c r="K36" s="3">
         <v>20</v>
       </c>
-      <c r="L36" s="2">
+      <c r="L36" s="3">
         <v>12009</v>
       </c>
-      <c r="M36" s="2">
+      <c r="M36" s="3">
         <v>246592.80600000001</v>
       </c>
-      <c r="N36">
+      <c r="N36" s="3">
         <v>644</v>
       </c>
-      <c r="O36">
+      <c r="O36" s="3">
         <v>15</v>
       </c>
-      <c r="P36">
+      <c r="P36" s="3">
         <v>77</v>
       </c>
-      <c r="Q36">
+      <c r="Q36" s="3">
         <v>2654</v>
       </c>
-      <c r="R36">
+      <c r="R36" s="3">
         <v>0.27</v>
       </c>
-      <c r="S36">
+      <c r="S36" s="3">
         <v>0.11</v>
       </c>
-      <c r="T36">
+      <c r="T36" s="3">
         <v>0.39</v>
       </c>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2" t="s">
+      <c r="D37" s="3"/>
+      <c r="E37" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G37" s="3">
         <v>12</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="3">
         <v>6.64</v>
       </c>
-      <c r="I37" s="2">
+      <c r="I37" s="3">
         <v>1.38</v>
       </c>
-      <c r="J37" s="2">
+      <c r="J37" s="3">
         <v>3.95</v>
       </c>
-      <c r="K37" s="2">
+      <c r="K37" s="3">
         <v>20</v>
       </c>
-      <c r="L37" s="2">
+      <c r="L37" s="3">
         <v>9596</v>
       </c>
-      <c r="M37" s="2">
+      <c r="M37" s="3">
         <v>127607.60799999999</v>
       </c>
-      <c r="N37">
+      <c r="N37" s="3">
         <v>595</v>
       </c>
-      <c r="O37">
+      <c r="O37" s="3">
         <v>10</v>
       </c>
-      <c r="P37">
+      <c r="P37" s="3">
         <v>78</v>
       </c>
-      <c r="Q37">
+      <c r="Q37" s="3">
         <v>1381</v>
       </c>
-      <c r="R37">
+      <c r="R37" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="S37">
+      <c r="S37" s="3">
         <v>0.2</v>
       </c>
-      <c r="T37">
+      <c r="T37" s="3">
         <v>0.48</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="D38" s="3"/>
-      <c r="E38" s="2" t="s">
+      <c r="D38" s="1"/>
+      <c r="E38" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38" s="3">
         <v>12</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38" s="3">
         <v>6.83</v>
       </c>
-      <c r="I38" s="2">
+      <c r="I38" s="3">
         <v>1.41</v>
       </c>
-      <c r="J38" s="2">
+      <c r="J38" s="3">
         <v>0.52</v>
       </c>
-      <c r="K38" s="2">
+      <c r="K38" s="3">
         <v>20</v>
       </c>
-      <c r="L38" s="2">
+      <c r="L38" s="3">
         <v>13499</v>
       </c>
-      <c r="M38" s="2">
+      <c r="M38" s="3">
         <v>136690.87399999899</v>
       </c>
-      <c r="N38">
+      <c r="N38" s="3">
         <v>729</v>
       </c>
-      <c r="O38">
+      <c r="O38" s="3">
         <v>15</v>
       </c>
-      <c r="P38">
+      <c r="P38" s="3">
         <v>81</v>
       </c>
-      <c r="Q38">
+      <c r="Q38" s="3">
         <v>2990</v>
       </c>
-      <c r="R38">
+      <c r="R38" s="3">
         <v>0.3</v>
       </c>
-      <c r="S38">
+      <c r="S38" s="3">
         <v>0.22</v>
       </c>
-      <c r="T38">
+      <c r="T38" s="3">
         <v>0.4</v>
       </c>
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="C39" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="2" t="s">
+      <c r="D39" s="1"/>
+      <c r="E39" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39" s="3">
         <v>12</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39" s="3">
         <v>5.16</v>
       </c>
-      <c r="I39" s="2">
+      <c r="I39" s="3">
         <v>0.88</v>
       </c>
-      <c r="J39" s="2">
+      <c r="J39" s="3">
         <v>2.96</v>
       </c>
-      <c r="K39" s="2">
+      <c r="K39" s="3">
         <v>20</v>
       </c>
-      <c r="L39" s="2">
+      <c r="L39" s="3">
         <v>11262</v>
       </c>
-      <c r="M39" s="2">
+      <c r="M39" s="3">
         <v>112980.38400000001</v>
       </c>
-      <c r="N39">
+      <c r="N39" s="3">
         <v>114</v>
       </c>
-      <c r="O39">
+      <c r="O39" s="3">
         <v>15</v>
       </c>
-      <c r="P39">
+      <c r="P39" s="3">
         <v>75</v>
       </c>
-      <c r="Q39">
+      <c r="Q39" s="3">
         <v>980</v>
       </c>
-      <c r="R39">
+      <c r="R39" s="3">
         <v>0.18</v>
       </c>
-      <c r="S39">
+      <c r="S39" s="3">
         <v>0.2</v>
       </c>
-      <c r="T39">
+      <c r="T39" s="3">
         <v>0.45</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="D40" s="3"/>
+      <c r="E40" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40" s="3">
         <v>26</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40" s="3">
         <v>2.25</v>
       </c>
-      <c r="I40" s="2">
+      <c r="I40" s="3">
         <v>0.6</v>
       </c>
-      <c r="J40" s="2">
+      <c r="J40" s="3">
         <v>8.9</v>
       </c>
-      <c r="K40" s="2">
+      <c r="K40" s="3">
         <v>50</v>
       </c>
-      <c r="L40" s="2">
+      <c r="L40" s="3">
         <v>14407</v>
       </c>
-      <c r="M40" s="2">
+      <c r="M40" s="3">
         <v>185490.125</v>
       </c>
-      <c r="N40">
+      <c r="N40" s="3">
         <v>683</v>
       </c>
-      <c r="O40">
+      <c r="O40" s="3">
         <v>15</v>
       </c>
-      <c r="P40">
+      <c r="P40" s="3">
         <v>92</v>
       </c>
-      <c r="Q40">
+      <c r="Q40" s="3">
         <v>2490</v>
       </c>
-      <c r="R40">
+      <c r="R40" s="3">
         <v>0.23</v>
       </c>
-      <c r="S40">
+      <c r="S40" s="3">
         <v>0.23</v>
       </c>
-      <c r="T40">
+      <c r="T40" s="3">
         <v>0.2</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="3">
         <v>84189990</v>
       </c>
-      <c r="E41" s="2" t="s">
+      <c r="E41" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="3">
         <v>12</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="3">
         <v>12.36</v>
       </c>
-      <c r="I41" s="2">
+      <c r="I41" s="3">
         <v>1.1499999999999999</v>
       </c>
-      <c r="J41" s="2">
+      <c r="J41" s="3">
         <v>1.48</v>
       </c>
-      <c r="K41" s="2">
+      <c r="K41" s="3">
         <v>20</v>
       </c>
-      <c r="L41" s="2">
+      <c r="L41" s="3">
         <v>6208</v>
       </c>
-      <c r="M41" s="2">
+      <c r="M41" s="3">
         <v>108404.095999999</v>
       </c>
-      <c r="N41">
+      <c r="N41" s="3">
         <v>466</v>
       </c>
-      <c r="O41">
+      <c r="O41" s="3">
         <v>20</v>
       </c>
-      <c r="P41">
+      <c r="P41" s="3">
         <v>75</v>
       </c>
-      <c r="Q41">
+      <c r="Q41" s="3">
         <v>2925</v>
       </c>
-      <c r="R41">
+      <c r="R41" s="3">
         <v>0.28000000000000003</v>
       </c>
-      <c r="S41">
+      <c r="S41" s="3">
         <v>0.18</v>
       </c>
-      <c r="T41">
+      <c r="T41" s="3">
         <v>0.26</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D42" s="3"/>
-      <c r="E42" s="2" t="s">
+      <c r="D42" s="1"/>
+      <c r="E42" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="3">
         <v>12</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="3">
         <v>5.58</v>
       </c>
-      <c r="I42" s="2">
+      <c r="I42" s="3">
         <v>1.19</v>
       </c>
-      <c r="J42" s="2">
+      <c r="J42" s="3">
         <v>0.7</v>
       </c>
-      <c r="K42" s="2">
+      <c r="K42" s="3">
         <v>20</v>
       </c>
-      <c r="L42" s="2">
+      <c r="L42" s="3">
         <v>13226</v>
       </c>
-      <c r="M42" s="2">
+      <c r="M42" s="3">
         <v>113558.436</v>
       </c>
-      <c r="N42">
+      <c r="N42" s="3">
         <v>348</v>
       </c>
-      <c r="O42">
+      <c r="O42" s="3">
         <v>10</v>
       </c>
-      <c r="P42">
+      <c r="P42" s="3">
         <v>76</v>
       </c>
-      <c r="Q42">
+      <c r="Q42" s="3">
         <v>516</v>
       </c>
-      <c r="R42">
+      <c r="R42" s="3">
         <v>0.24</v>
       </c>
-      <c r="S42">
+      <c r="S42" s="3">
         <v>0.23</v>
       </c>
-      <c r="T42">
+      <c r="T42" s="3">
         <v>0.32</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="C43" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2" t="s">
+      <c r="D43" s="3"/>
+      <c r="E43" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43" s="3">
         <v>32</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="3">
         <v>4.8499999999999996</v>
       </c>
-      <c r="I43" s="2">
+      <c r="I43" s="3">
         <v>1.03</v>
       </c>
-      <c r="J43" s="2">
+      <c r="J43" s="3">
         <v>2.66</v>
       </c>
-      <c r="K43" s="2">
+      <c r="K43" s="3">
         <v>25</v>
       </c>
-      <c r="L43" s="2">
+      <c r="L43" s="3">
         <v>9847</v>
       </c>
-      <c r="M43" s="2">
+      <c r="M43" s="3">
         <v>96032.867499999993</v>
       </c>
-      <c r="N43">
+      <c r="N43" s="3">
         <v>677</v>
       </c>
-      <c r="O43">
+      <c r="O43" s="3">
         <v>15</v>
       </c>
-      <c r="P43">
+      <c r="P43" s="3">
         <v>83</v>
       </c>
-      <c r="Q43">
+      <c r="Q43" s="3">
         <v>1308</v>
       </c>
-      <c r="R43">
+      <c r="R43" s="3">
         <v>0.26</v>
       </c>
-      <c r="S43">
+      <c r="S43" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="T43">
+      <c r="T43" s="3">
         <v>0.34</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C44" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="D44" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="E44" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G44" s="3">
         <v>32</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44" s="3">
         <v>14.47</v>
       </c>
-      <c r="I44" s="2">
+      <c r="I44" s="3">
         <v>0.78</v>
       </c>
-      <c r="J44" s="2">
+      <c r="J44" s="3">
         <v>0.91</v>
       </c>
-      <c r="K44" s="2">
+      <c r="K44" s="3">
         <v>25</v>
       </c>
-      <c r="L44" s="2">
+      <c r="L44" s="3">
         <v>5611</v>
       </c>
-      <c r="M44" s="2">
+      <c r="M44" s="3">
         <v>110971.552499999</v>
       </c>
-      <c r="N44">
+      <c r="N44" s="3">
         <v>615</v>
       </c>
-      <c r="O44">
+      <c r="O44" s="3">
         <v>15</v>
       </c>
-      <c r="P44">
+      <c r="P44" s="3">
         <v>80</v>
       </c>
-      <c r="Q44">
+      <c r="Q44" s="3">
         <v>1974</v>
       </c>
-      <c r="R44">
+      <c r="R44" s="3">
         <v>0.14000000000000001</v>
       </c>
-      <c r="S44">
+      <c r="S44" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="T44">
+      <c r="T44" s="3">
         <v>0.45</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C45" s="3" t="s">
+      <c r="C45" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="D45" s="3"/>
-      <c r="E45" s="2" t="s">
+      <c r="D45" s="1"/>
+      <c r="E45" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F45" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G45" s="3">
         <v>26</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H45" s="3">
         <v>4.25</v>
       </c>
-      <c r="I45" s="2">
+      <c r="I45" s="3">
         <v>0.89</v>
       </c>
-      <c r="J45" s="2">
+      <c r="J45" s="3">
         <v>3.08</v>
       </c>
-      <c r="K45" s="2">
+      <c r="K45" s="3">
         <v>50</v>
       </c>
-      <c r="L45" s="2">
+      <c r="L45" s="3">
         <v>2854</v>
       </c>
-      <c r="M45" s="2">
+      <c r="M45" s="3">
         <v>29524.629999999899</v>
       </c>
-      <c r="N45">
+      <c r="N45" s="3">
         <v>502</v>
       </c>
-      <c r="O45">
+      <c r="O45" s="3">
         <v>20</v>
       </c>
-      <c r="P45">
+      <c r="P45" s="3">
         <v>84</v>
       </c>
-      <c r="Q45">
+      <c r="Q45" s="3">
         <v>2895</v>
       </c>
-      <c r="R45">
+      <c r="R45" s="3">
         <v>0.26</v>
       </c>
-      <c r="S45">
+      <c r="S45" s="3">
         <v>0.17</v>
       </c>
-      <c r="T45">
+      <c r="T45" s="3">
         <v>0.41</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D46" s="2"/>
-      <c r="E46" s="2" t="s">
+      <c r="D46" s="3"/>
+      <c r="E46" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G46" s="3">
         <v>26</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H46" s="3">
         <v>8.1199999999999992</v>
       </c>
-      <c r="I46" s="2">
+      <c r="I46" s="3">
         <v>1.1499999999999999</v>
       </c>
-      <c r="J46" s="2">
+      <c r="J46" s="3">
         <v>14.56</v>
       </c>
-      <c r="K46" s="2">
+      <c r="K46" s="3">
         <v>50</v>
       </c>
-      <c r="L46" s="2">
+      <c r="L46" s="3">
         <v>17330</v>
       </c>
-      <c r="M46" s="2">
+      <c r="M46" s="3">
         <v>483333.7</v>
       </c>
-      <c r="N46">
+      <c r="N46" s="3">
         <v>395</v>
       </c>
-      <c r="O46">
+      <c r="O46" s="3">
         <v>20</v>
       </c>
-      <c r="P46">
+      <c r="P46" s="3">
         <v>83</v>
       </c>
-      <c r="Q46">
+      <c r="Q46" s="3">
         <v>2546</v>
       </c>
-      <c r="R46">
+      <c r="R46" s="3">
         <v>0.34</v>
       </c>
-      <c r="S46">
+      <c r="S46" s="3">
         <v>0.21</v>
       </c>
-      <c r="T46">
+      <c r="T46" s="3">
         <v>0.35</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2" t="s">
+      <c r="D47" s="3"/>
+      <c r="E47" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G47" s="3">
         <v>26</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47" s="3">
         <v>9.69</v>
       </c>
-      <c r="I47" s="2">
+      <c r="I47" s="3">
         <v>1.25</v>
       </c>
-      <c r="J47" s="2">
+      <c r="J47" s="3">
         <v>11.99</v>
       </c>
-      <c r="K47" s="2">
+      <c r="K47" s="3">
         <v>50</v>
       </c>
-      <c r="L47" s="2">
+      <c r="L47" s="3">
         <v>27162</v>
       </c>
-      <c r="M47" s="2">
+      <c r="M47" s="3">
         <v>754424.549999999</v>
       </c>
-      <c r="N47">
+      <c r="N47" s="3">
         <v>723</v>
       </c>
-      <c r="O47">
+      <c r="O47" s="3">
         <v>10</v>
       </c>
-      <c r="P47">
+      <c r="P47" s="3">
         <v>94</v>
       </c>
-      <c r="Q47">
+      <c r="Q47" s="3">
         <v>2983</v>
       </c>
-      <c r="R47">
+      <c r="R47" s="3">
         <v>0.33</v>
       </c>
-      <c r="S47">
+      <c r="S47" s="3">
         <v>0.22</v>
       </c>
-      <c r="T47">
+      <c r="T47" s="3">
         <v>0.44</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="D48" s="2"/>
-      <c r="E48" s="2" t="s">
+      <c r="D48" s="3"/>
+      <c r="E48" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F48" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G48" s="3">
         <v>26</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H48" s="3">
         <v>8.16</v>
       </c>
-      <c r="I48" s="2">
+      <c r="I48" s="3">
         <v>0.56999999999999995</v>
       </c>
-      <c r="J48" s="2">
+      <c r="J48" s="3">
         <v>3.52</v>
       </c>
-      <c r="K48" s="2">
+      <c r="K48" s="3">
         <v>50</v>
       </c>
-      <c r="L48" s="2">
+      <c r="L48" s="3">
         <v>29989</v>
       </c>
-      <c r="M48" s="2">
+      <c r="M48" s="3">
         <v>489720.37</v>
       </c>
-      <c r="N48">
+      <c r="N48" s="3">
         <v>226</v>
       </c>
-      <c r="O48">
+      <c r="O48" s="3">
         <v>20</v>
       </c>
-      <c r="P48">
+      <c r="P48" s="3">
         <v>77</v>
       </c>
-      <c r="Q48">
+      <c r="Q48" s="3">
         <v>2523</v>
       </c>
-      <c r="R48">
+      <c r="R48" s="3">
         <v>0.17</v>
       </c>
-      <c r="S48">
+      <c r="S48" s="3">
         <v>0.28000000000000003</v>
       </c>
-      <c r="T48">
+      <c r="T48" s="3">
         <v>0.34</v>
       </c>
     </row>
     <row r="49" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="3">
         <v>84189990</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E49" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F49" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="G49" s="2">
+      <c r="G49" s="3">
         <v>32</v>
       </c>
-      <c r="H49" s="2">
+      <c r="H49" s="3">
         <v>12.52</v>
       </c>
-      <c r="I49" s="2">
+      <c r="I49" s="3">
         <v>1.0900000000000001</v>
       </c>
-      <c r="J49" s="2">
+      <c r="J49" s="3">
         <v>4.9400000000000004</v>
       </c>
-      <c r="K49" s="2">
+      <c r="K49" s="3">
         <v>25</v>
       </c>
-      <c r="L49" s="2">
+      <c r="L49" s="3">
         <v>8822</v>
       </c>
-      <c r="M49" s="2">
+      <c r="M49" s="3">
         <v>191260.96</v>
       </c>
-      <c r="N49">
+      <c r="N49" s="3">
         <v>218</v>
       </c>
-      <c r="O49">
+      <c r="O49" s="3">
         <v>10</v>
       </c>
-      <c r="P49">
+      <c r="P49" s="3">
         <v>92</v>
       </c>
-      <c r="Q49">
+      <c r="Q49" s="3">
         <v>1045</v>
       </c>
-      <c r="R49">
+      <c r="R49" s="3">
         <v>0.13</v>
       </c>
-      <c r="S49">
+      <c r="S49" s="3">
         <v>0.16</v>
       </c>
-      <c r="T49">
+      <c r="T49" s="3">
         <v>0.24</v>
       </c>
     </row>
     <row r="50" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2" t="s">
+      <c r="D50" s="3"/>
+      <c r="E50" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="F50" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="G50" s="2">
+      <c r="G50" s="3">
         <v>32</v>
       </c>
-      <c r="H50" s="2">
+      <c r="H50" s="3">
         <v>10.34</v>
       </c>
-      <c r="I50" s="2">
+      <c r="I50" s="3">
         <v>0.71</v>
       </c>
-      <c r="J50" s="2">
+      <c r="J50" s="3">
         <v>3.76</v>
       </c>
-      <c r="K50" s="2">
+      <c r="K50" s="3">
         <v>25</v>
       </c>
-      <c r="L50" s="2">
+      <c r="L50" s="3">
         <v>6192</v>
       </c>
-      <c r="M50" s="2">
+      <c r="M50" s="3">
         <v>107709.84</v>
       </c>
-      <c r="N50">
+      <c r="N50" s="3">
         <v>589</v>
       </c>
-      <c r="O50">
+      <c r="O50" s="3">
         <v>15</v>
       </c>
-      <c r="P50">
+      <c r="P50" s="3">
         <v>89</v>
       </c>
-      <c r="Q50">
+      <c r="Q50" s="3">
         <v>2325</v>
       </c>
-      <c r="R50">
+      <c r="R50" s="3">
         <v>0.18</v>
       </c>
-      <c r="S50">
+      <c r="S50" s="3">
         <v>0.21</v>
       </c>
-      <c r="T50">
+      <c r="T50" s="3">
         <v>0.41</v>
       </c>
     </row>
     <row r="51" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E51" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="F51" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G51" s="2">
+      <c r="G51" s="3">
         <v>32</v>
       </c>
-      <c r="H51" s="2">
+      <c r="H51" s="3">
         <v>6.15</v>
       </c>
-      <c r="I51" s="2">
+      <c r="I51" s="3">
         <v>1.1499999999999999</v>
       </c>
-      <c r="J51" s="2">
+      <c r="J51" s="3">
         <v>7.09</v>
       </c>
-      <c r="K51" s="2">
+      <c r="K51" s="3">
         <v>25</v>
       </c>
-      <c r="L51" s="2">
+      <c r="L51" s="3">
         <v>23929</v>
       </c>
-      <c r="M51" s="2">
+      <c r="M51" s="3">
         <v>381129.14750000002</v>
       </c>
-      <c r="N51">
+      <c r="N51" s="3">
         <v>546</v>
       </c>
-      <c r="O51">
+      <c r="O51" s="3">
         <v>15</v>
       </c>
-      <c r="P51">
+      <c r="P51" s="3">
         <v>94</v>
       </c>
-      <c r="Q51">
+      <c r="Q51" s="3">
         <v>2995</v>
       </c>
-      <c r="R51">
+      <c r="R51" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="S51">
+      <c r="S51" s="3">
         <v>0.13</v>
       </c>
-      <c r="T51">
+      <c r="T51" s="3">
         <v>0.25</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T51" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>